<commit_message>
auto backup 2022-08-06 23:39:07.279755
</commit_message>
<xml_diff>
--- a/walla_ads_file.xlsx
+++ b/walla_ads_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBook\OneDrive\A_Miscalaneus\Escritorio\Code\git_folder\walla_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFF610C-7B2C-4361-9C73-00E39E3C31ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A4FEB-3160-4BAA-A32D-BFFC0580FBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10910" yWindow="-1800" windowWidth="11020" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -211,12 +211,6 @@
     <t>SubCategoria 2</t>
   </si>
   <si>
-    <t>Peso</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>Marca</t>
   </si>
   <si>
@@ -310,9 +304,6 @@
     <t xml:space="preserve">iphone SE 2022 64GB </t>
   </si>
   <si>
-    <t>iphone iphone SE 2022 negro _ad1.jpg,iphone iphone SE 2022 todos _ad2.jpg,img3 icons.jpg,layout 4.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">iphone SE 2022 64 </t>
   </si>
   <si>
@@ -325,12 +316,6 @@
     <t>iphone</t>
   </si>
   <si>
-    <t>móviles</t>
-  </si>
-  <si>
-    <t>teléfonos móviles</t>
-  </si>
-  <si>
     <t>Consolas y Videojuegos</t>
   </si>
   <si>
@@ -419,6 +404,21 @@
   </si>
   <si>
     <t>⭐️ Smart-Market.es ⭐️ En nuestra tienda Online ✅ encontrarás fotos reales de cada artículo ✅ además de muchos más precios y modelos ✅ | Te deseamos Feliz Compra 💯| Visita Smart-market.es |</t>
+  </si>
+  <si>
+    <t>Peso | 2, 5, 10, 20, 30 (kg)</t>
+  </si>
+  <si>
+    <t>Móviles y Telefonía</t>
+  </si>
+  <si>
+    <t>Teléfonos móviles</t>
+  </si>
+  <si>
+    <t>Estado | Sin Abrir, Nuevo,  Como nuevo,  En buen estado</t>
+  </si>
+  <si>
+    <t>iphone SE 2022 negro _ad1.jpg,iphone SE 2022 todos _ad2.jpg,img3 icons.jpg,layout 4.jpg</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -956,59 +956,61 @@
         <v>62</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="Q1" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="O2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q2" s="2">
         <v>629</v>
@@ -1016,31 +1018,31 @@
     </row>
     <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="I3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>1</v>
@@ -1051,34 +1053,34 @@
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="Q4">
         <v>130</v>
@@ -1086,31 +1088,31 @@
     </row>
     <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>3</v>
@@ -1121,31 +1123,31 @@
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>4</v>
@@ -1156,31 +1158,31 @@
     </row>
     <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="O7" t="s">
         <v>6</v>
@@ -1191,31 +1193,31 @@
     </row>
     <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G8" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="O8" t="s">
         <v>7</v>
@@ -1226,32 +1228,32 @@
     </row>
     <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G9" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>10</v>
@@ -1262,31 +1264,31 @@
     </row>
     <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G10" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>12</v>
@@ -1294,31 +1296,31 @@
     </row>
     <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O11" t="s">
         <v>14</v>
@@ -1326,31 +1328,31 @@
     </row>
     <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J12" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s">
+        <v>97</v>
+      </c>
+      <c r="L12" t="s">
         <v>105</v>
-      </c>
-      <c r="K12" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" t="s">
-        <v>110</v>
       </c>
       <c r="O12" t="s">
         <v>16</v>
@@ -1358,31 +1360,31 @@
     </row>
     <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="O13" t="s">
         <v>17</v>
@@ -1390,31 +1392,31 @@
     </row>
     <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="O14" t="s">
         <v>19</v>
@@ -1422,31 +1424,31 @@
     </row>
     <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G15" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L15" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="O15" t="s">
         <v>21</v>
@@ -1454,31 +1456,31 @@
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J16" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="O16" t="s">
         <v>22</v>
@@ -1486,31 +1488,31 @@
     </row>
     <row r="17" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G17" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L17" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="O17" t="s">
         <v>23</v>
@@ -1518,31 +1520,31 @@
     </row>
     <row r="18" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G18" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="O18" t="s">
         <v>24</v>
@@ -1550,31 +1552,31 @@
     </row>
     <row r="19" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="O19" t="s">
         <v>26</v>
@@ -1582,31 +1584,31 @@
     </row>
     <row r="20" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G20" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="O20" t="s">
         <v>28</v>
@@ -1614,95 +1616,95 @@
     </row>
     <row r="21" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F21" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G21" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J21" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="O22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="G23" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="I23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="O23" t="s">
         <v>29</v>
@@ -1713,23 +1715,23 @@
         <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" t="s">
         <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I24" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L24" t="s">
         <v>30</v>
@@ -1743,23 +1745,23 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" t="s">
         <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J25" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L25" t="s">
         <v>32</v>
@@ -1773,23 +1775,23 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" t="s">
         <v>34</v>
       </c>
       <c r="F26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L26" t="s">
         <v>33</v>
@@ -1803,23 +1805,23 @@
         <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" t="s">
         <v>36</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J27" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L27" t="s">
         <v>35</v>
@@ -1833,23 +1835,23 @@
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" t="s">
         <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L28" t="s">
         <v>37</v>
@@ -1863,23 +1865,23 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" t="s">
         <v>40</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>39</v>
@@ -1893,23 +1895,23 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" t="s">
         <v>42</v>
       </c>
       <c r="F30" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J30" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L30" t="s">
         <v>41</v>
@@ -1923,23 +1925,23 @@
         <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" t="s">
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J31" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L31" t="s">
         <v>43</v>
@@ -1953,23 +1955,23 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" t="s">
         <v>46</v>
       </c>
       <c r="F32" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G32" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J32" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L32" t="s">
         <v>45</v>
@@ -1983,23 +1985,23 @@
         <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" t="s">
         <v>48</v>
       </c>
       <c r="F33" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J33" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L33" t="s">
         <v>47</v>
@@ -2013,23 +2015,23 @@
         <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" t="s">
         <v>50</v>
       </c>
       <c r="F34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J34" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L34" t="s">
         <v>49</v>
@@ -2043,23 +2045,23 @@
         <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" t="s">
         <v>52</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L35" t="s">
         <v>51</v>
@@ -2073,23 +2075,23 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" t="s">
         <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L36" t="s">
         <v>53</v>
@@ -2103,23 +2105,23 @@
         <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" t="s">
         <v>52</v>
       </c>
       <c r="F37" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G37" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J37" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L37" t="s">
         <v>51</v>
@@ -2133,23 +2135,23 @@
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" t="s">
         <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G38" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J38" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L38" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
updated bot, added prods NOT uploaded because of error
</commit_message>
<xml_diff>
--- a/walla_ads_file.xlsx
+++ b/walla_ads_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBook\OneDrive\A_Miscalaneus\Escritorio\Code\git_folder\walla_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A4FEB-3160-4BAA-A32D-BFFC0580FBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191C58B-0649-4176-9BDE-3CE1B43DB252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="134">
   <si>
     <t>iphone se 2020 rojo _ad1.jpg,iphone se 2020 todos _ad2.jpg,img3 icons.jpg,layout 4.jpg</t>
   </si>
@@ -253,9 +253,6 @@
     <t xml:space="preserve">iphone 13 pro max 128GB </t>
   </si>
   <si>
-    <t xml:space="preserve">iphone 13 pro 128GB </t>
-  </si>
-  <si>
     <t xml:space="preserve">iphone 11 PRO MAX 64GB  </t>
   </si>
   <si>
@@ -403,9 +400,6 @@
     <t xml:space="preserve">iphone 7 64 GB  </t>
   </si>
   <si>
-    <t>⭐️ Smart-Market.es ⭐️ En nuestra tienda Online ✅ encontrarás fotos reales de cada artículo ✅ además de muchos más precios y modelos ✅ | Te deseamos Feliz Compra 💯| Visita Smart-market.es |</t>
-  </si>
-  <si>
     <t>Peso | 2, 5, 10, 20, 30 (kg)</t>
   </si>
   <si>
@@ -419,6 +413,23 @@
   </si>
   <si>
     <t>iphone SE 2022 negro _ad1.jpg,iphone SE 2022 todos _ad2.jpg,img3 icons.jpg,layout 4.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⭐️ Smart-Market⭐️ 
+Todos Nuestros artículos cuenta con grantía de hasta 2 años 👌
+Con factura de compra 📖
+Te damos perído de prueba o devolución 😊
+Puedes ver fotos reales del artículo 📸
+Envío Gratis! 🚚
+Te desamos feliz compra 💯
+Referencia de anuncio: AX233
+⭐️ Smart-Market⭐️ </t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>iphone 11 pro max verde _ad1.jpg,iphone 11 pro max gris _ad2.jpg,layout 2 no link.jpg,imagen 4 logo sin link.jpg</t>
   </si>
 </sst>
 </file>
@@ -515,7 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -525,6 +536,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent5" xfId="2" builtinId="48"/>
@@ -910,11 +924,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -956,10 +970,10 @@
         <v>62</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>63</v>
@@ -974,43 +988,42 @@
         <v>66</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2">
+        <v>499</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="O2" t="s">
         <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="2">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
-        <v>101</v>
-      </c>
-      <c r="O2" t="s">
-        <v>94</v>
       </c>
       <c r="Q2" s="2">
         <v>629</v>
@@ -1018,28 +1031,31 @@
     </row>
     <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3">
+        <v>599</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>127</v>
       </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>129</v>
-      </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K3" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>102</v>
@@ -1052,68 +1068,44 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4">
+        <v>314</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>127</v>
       </c>
-      <c r="E4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F4" t="s">
-        <v>129</v>
-      </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L4" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="Q4">
         <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" t="s">
-        <v>130</v>
-      </c>
-      <c r="I5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" t="s">
-        <v>100</v>
-      </c>
-      <c r="K5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="O5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1122,33 +1114,6 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G6" t="s">
-        <v>130</v>
-      </c>
-      <c r="I6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="O6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1160,29 +1125,29 @@
       <c r="B7" t="s">
         <v>67</v>
       </c>
-      <c r="C7" t="s">
-        <v>127</v>
+      <c r="C7" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K7" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O7" t="s">
         <v>6</v>
@@ -1195,29 +1160,29 @@
       <c r="B8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
-        <v>127</v>
+      <c r="C8" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K8" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O8" t="s">
         <v>7</v>
@@ -1230,30 +1195,30 @@
       <c r="B9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C9" t="s">
-        <v>127</v>
+      <c r="C9" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>10</v>
@@ -1263,33 +1228,6 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J10" t="s">
-        <v>100</v>
-      </c>
-      <c r="K10" t="s">
-        <v>97</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="O10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1298,93 +1236,66 @@
       <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" t="s">
-        <v>127</v>
+      <c r="C11" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K11" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" t="s">
-        <v>130</v>
-      </c>
-      <c r="I12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J12" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" t="s">
-        <v>105</v>
-      </c>
       <c r="O12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>127</v>
       </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" t="s">
-        <v>129</v>
-      </c>
       <c r="G13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K13" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O13" t="s">
         <v>17</v>
@@ -1392,31 +1303,31 @@
     </row>
     <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
-        <v>127</v>
+        <v>79</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K14" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O14" t="s">
         <v>19</v>
@@ -1426,29 +1337,29 @@
       <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
-        <v>127</v>
+      <c r="C15" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K15" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O15" t="s">
         <v>21</v>
@@ -1456,31 +1367,31 @@
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" t="s">
         <v>81</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
         <v>127</v>
       </c>
-      <c r="E16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" t="s">
-        <v>129</v>
-      </c>
       <c r="G16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K16" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O16" t="s">
         <v>22</v>
@@ -1488,31 +1399,31 @@
     </row>
     <row r="17" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>127</v>
       </c>
-      <c r="E17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" t="s">
-        <v>129</v>
-      </c>
       <c r="G17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K17" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O17" t="s">
         <v>23</v>
@@ -1520,31 +1431,31 @@
     </row>
     <row r="18" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" t="s">
         <v>85</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
         <v>127</v>
       </c>
-      <c r="E18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" t="s">
-        <v>129</v>
-      </c>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K18" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O18" t="s">
         <v>24</v>
@@ -1552,31 +1463,31 @@
     </row>
     <row r="19" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" t="s">
-        <v>127</v>
+        <v>90</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K19" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O19" t="s">
         <v>26</v>
@@ -1584,31 +1495,31 @@
     </row>
     <row r="20" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>127</v>
+        <v>91</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K20" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O20" t="s">
         <v>28</v>
@@ -1616,95 +1527,95 @@
     </row>
     <row r="21" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
         <v>127</v>
       </c>
-      <c r="E21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" t="s">
-        <v>129</v>
-      </c>
       <c r="G21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K21" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
         <v>127</v>
       </c>
-      <c r="E22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" t="s">
-        <v>129</v>
-      </c>
       <c r="G22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K22" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
         <v>127</v>
       </c>
-      <c r="E23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" t="s">
-        <v>129</v>
-      </c>
       <c r="G23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K23" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="L23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O23" t="s">
         <v>29</v>
@@ -1714,24 +1625,24 @@
       <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
-        <v>127</v>
+      <c r="C24" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" t="s">
         <v>31</v>
       </c>
       <c r="F24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" t="s">
         <v>98</v>
       </c>
-      <c r="G24" t="s">
-        <v>99</v>
-      </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L24" t="s">
         <v>30</v>
@@ -1744,24 +1655,24 @@
       <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="C25" t="s">
-        <v>127</v>
+      <c r="C25" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" t="s">
         <v>31</v>
       </c>
       <c r="F25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" t="s">
         <v>98</v>
       </c>
-      <c r="G25" t="s">
-        <v>99</v>
-      </c>
       <c r="I25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L25" t="s">
         <v>32</v>
@@ -1774,24 +1685,24 @@
       <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="C26" t="s">
-        <v>127</v>
+      <c r="C26" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" t="s">
         <v>34</v>
       </c>
       <c r="F26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" t="s">
         <v>98</v>
       </c>
-      <c r="G26" t="s">
-        <v>99</v>
-      </c>
       <c r="I26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L26" t="s">
         <v>33</v>
@@ -1804,24 +1715,24 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="s">
-        <v>127</v>
+      <c r="C27" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" t="s">
         <v>36</v>
       </c>
       <c r="F27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" t="s">
         <v>98</v>
       </c>
-      <c r="G27" t="s">
-        <v>99</v>
-      </c>
       <c r="I27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L27" t="s">
         <v>35</v>
@@ -1834,24 +1745,24 @@
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" t="s">
-        <v>127</v>
+      <c r="C28" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" t="s">
         <v>38</v>
       </c>
       <c r="F28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" t="s">
         <v>98</v>
       </c>
-      <c r="G28" t="s">
-        <v>99</v>
-      </c>
       <c r="I28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L28" t="s">
         <v>37</v>
@@ -1864,24 +1775,24 @@
       <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C29" t="s">
-        <v>127</v>
+      <c r="C29" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" t="s">
         <v>40</v>
       </c>
       <c r="F29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" t="s">
         <v>98</v>
       </c>
-      <c r="G29" t="s">
-        <v>99</v>
-      </c>
       <c r="I29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>39</v>
@@ -1894,24 +1805,24 @@
       <c r="B30" t="s">
         <v>41</v>
       </c>
-      <c r="C30" t="s">
-        <v>127</v>
+      <c r="C30" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" t="s">
         <v>42</v>
       </c>
       <c r="F30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" t="s">
         <v>98</v>
       </c>
-      <c r="G30" t="s">
-        <v>99</v>
-      </c>
       <c r="I30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L30" t="s">
         <v>41</v>
@@ -1924,24 +1835,24 @@
       <c r="B31" t="s">
         <v>43</v>
       </c>
-      <c r="C31" t="s">
-        <v>127</v>
+      <c r="C31" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" t="s">
         <v>44</v>
       </c>
       <c r="F31" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" t="s">
         <v>98</v>
       </c>
-      <c r="G31" t="s">
-        <v>99</v>
-      </c>
       <c r="I31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L31" t="s">
         <v>43</v>
@@ -1954,24 +1865,24 @@
       <c r="B32" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
-        <v>127</v>
+      <c r="C32" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" t="s">
         <v>46</v>
       </c>
       <c r="F32" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" t="s">
         <v>98</v>
       </c>
-      <c r="G32" t="s">
-        <v>99</v>
-      </c>
       <c r="I32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L32" t="s">
         <v>45</v>
@@ -1980,28 +1891,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" t="s">
-        <v>127</v>
+      <c r="C33" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" t="s">
         <v>48</v>
       </c>
       <c r="F33" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" t="s">
         <v>98</v>
       </c>
-      <c r="G33" t="s">
-        <v>99</v>
-      </c>
       <c r="I33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L33" t="s">
         <v>47</v>
@@ -2010,28 +1921,28 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="C34" t="s">
-        <v>127</v>
+      <c r="C34" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" t="s">
         <v>50</v>
       </c>
       <c r="F34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" t="s">
         <v>98</v>
       </c>
-      <c r="G34" t="s">
-        <v>99</v>
-      </c>
       <c r="I34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L34" t="s">
         <v>49</v>
@@ -2040,28 +1951,28 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="C35" t="s">
-        <v>127</v>
+      <c r="C35" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" t="s">
         <v>52</v>
       </c>
       <c r="F35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" t="s">
         <v>98</v>
       </c>
-      <c r="G35" t="s">
-        <v>99</v>
-      </c>
       <c r="I35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L35" t="s">
         <v>51</v>
@@ -2070,28 +1981,28 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>53</v>
       </c>
-      <c r="C36" t="s">
-        <v>127</v>
+      <c r="C36" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" t="s">
         <v>54</v>
       </c>
       <c r="F36" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" t="s">
         <v>98</v>
       </c>
-      <c r="G36" t="s">
-        <v>99</v>
-      </c>
       <c r="I36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L36" t="s">
         <v>53</v>
@@ -2100,28 +2011,28 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>51</v>
       </c>
-      <c r="C37" t="s">
-        <v>127</v>
+      <c r="C37" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" t="s">
         <v>52</v>
       </c>
       <c r="F37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" t="s">
         <v>98</v>
       </c>
-      <c r="G37" t="s">
-        <v>99</v>
-      </c>
       <c r="I37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L37" t="s">
         <v>51</v>
@@ -2130,34 +2041,154 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
-        <v>127</v>
+      <c r="C38" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" t="s">
         <v>54</v>
       </c>
       <c r="F38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
         <v>98</v>
       </c>
-      <c r="G38" t="s">
-        <v>99</v>
-      </c>
       <c r="I38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L38" t="s">
         <v>53</v>
       </c>
       <c r="O38" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O41" t="s">
+        <v>92</v>
+      </c>
+      <c r="P41" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>20</v>
+      </c>
+      <c r="R41" t="s">
+        <v>130</v>
+      </c>
+      <c r="S41" t="s">
+        <v>127</v>
+      </c>
+      <c r="T41" t="s">
+        <v>128</v>
+      </c>
+      <c r="U41" s="2"/>
+      <c r="V41" t="s">
+        <v>94</v>
+      </c>
+      <c r="W41" t="s">
+        <v>99</v>
+      </c>
+      <c r="X41" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="P42" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R42" t="s">
+        <v>0</v>
+      </c>
+      <c r="S42" t="s">
+        <v>127</v>
+      </c>
+      <c r="T42" t="s">
+        <v>128</v>
+      </c>
+      <c r="V42" t="s">
+        <v>94</v>
+      </c>
+      <c r="W42" t="s">
+        <v>99</v>
+      </c>
+      <c r="X42" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="P43" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R43" t="s">
+        <v>121</v>
+      </c>
+      <c r="S43" t="s">
+        <v>127</v>
+      </c>
+      <c r="T43" t="s">
+        <v>128</v>
+      </c>
+      <c r="V43" t="s">
+        <v>94</v>
+      </c>
+      <c r="W43" t="s">
+        <v>99</v>
+      </c>
+      <c r="X43" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P44" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R44" t="s">
+        <v>2</v>
+      </c>
+      <c r="S44" t="s">
+        <v>127</v>
+      </c>
+      <c r="T44" t="s">
+        <v>128</v>
+      </c>
+      <c r="V44" t="s">
+        <v>94</v>
+      </c>
+      <c r="W44" t="s">
+        <v>99</v>
+      </c>
+      <c r="X44" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto backup 2022-09-21 20:50:22.719924
</commit_message>
<xml_diff>
--- a/walla_ads_file.xlsx
+++ b/walla_ads_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP EliteBook\OneDrive\A_Miscalaneus\Escritorio\Code\git_folder\walla_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191C58B-0649-4176-9BDE-3CE1B43DB252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8538C6C4-ECFB-4E81-A121-D1EB9140DEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,11 +924,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y44"/>
+  <dimension ref="A1:Y77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1122,33 +1122,6 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" t="s">
-        <v>128</v>
-      </c>
-      <c r="I7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" t="s">
-        <v>99</v>
-      </c>
-      <c r="K7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L7" t="s">
-        <v>115</v>
-      </c>
       <c r="O7" t="s">
         <v>6</v>
       </c>
@@ -1157,33 +1130,6 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" t="s">
-        <v>128</v>
-      </c>
-      <c r="I8" t="s">
-        <v>94</v>
-      </c>
-      <c r="J8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L8" t="s">
-        <v>116</v>
-      </c>
       <c r="O8" t="s">
         <v>7</v>
       </c>
@@ -1192,34 +1138,6 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" t="s">
-        <v>94</v>
-      </c>
-      <c r="J9" t="s">
-        <v>99</v>
-      </c>
-      <c r="K9" t="s">
-        <v>132</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="O9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1233,33 +1151,6 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" t="s">
-        <v>128</v>
-      </c>
-      <c r="I11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" t="s">
-        <v>99</v>
-      </c>
-      <c r="K11" t="s">
-        <v>132</v>
-      </c>
-      <c r="L11" t="s">
-        <v>103</v>
-      </c>
       <c r="O11" t="s">
         <v>14</v>
       </c>
@@ -1270,808 +1161,136 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" t="s">
-        <v>128</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" t="s">
-        <v>99</v>
-      </c>
-      <c r="K13" t="s">
-        <v>132</v>
-      </c>
-      <c r="L13" t="s">
-        <v>105</v>
-      </c>
       <c r="O13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14" t="s">
-        <v>99</v>
-      </c>
-      <c r="K14" t="s">
-        <v>132</v>
-      </c>
-      <c r="L14" t="s">
-        <v>106</v>
-      </c>
       <c r="O14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G15" t="s">
-        <v>128</v>
-      </c>
-      <c r="I15" t="s">
-        <v>94</v>
-      </c>
-      <c r="J15" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" t="s">
-        <v>132</v>
-      </c>
-      <c r="L15" t="s">
-        <v>107</v>
-      </c>
       <c r="O15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" t="s">
-        <v>127</v>
-      </c>
-      <c r="G16" t="s">
-        <v>128</v>
-      </c>
-      <c r="I16" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" t="s">
-        <v>99</v>
-      </c>
-      <c r="K16" t="s">
-        <v>132</v>
-      </c>
-      <c r="L16" t="s">
-        <v>108</v>
-      </c>
       <c r="O16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" t="s">
-        <v>127</v>
-      </c>
-      <c r="G17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I17" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" t="s">
-        <v>99</v>
-      </c>
-      <c r="K17" t="s">
-        <v>132</v>
-      </c>
-      <c r="L17" t="s">
-        <v>109</v>
-      </c>
+    <row r="17" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" t="s">
-        <v>128</v>
-      </c>
-      <c r="I18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" t="s">
-        <v>132</v>
-      </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
+    <row r="18" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G19" t="s">
-        <v>128</v>
-      </c>
-      <c r="I19" t="s">
-        <v>94</v>
-      </c>
-      <c r="J19" t="s">
-        <v>99</v>
-      </c>
-      <c r="K19" t="s">
-        <v>132</v>
-      </c>
-      <c r="L19" t="s">
-        <v>111</v>
-      </c>
+    <row r="19" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" t="s">
-        <v>128</v>
-      </c>
-      <c r="I20" t="s">
-        <v>94</v>
-      </c>
-      <c r="J20" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" t="s">
-        <v>132</v>
-      </c>
-      <c r="L20" t="s">
-        <v>112</v>
-      </c>
+    <row r="20" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" t="s">
-        <v>128</v>
-      </c>
-      <c r="I21" t="s">
-        <v>94</v>
-      </c>
-      <c r="J21" t="s">
-        <v>99</v>
-      </c>
-      <c r="K21" t="s">
-        <v>132</v>
-      </c>
-      <c r="L21" t="s">
-        <v>118</v>
-      </c>
+    <row r="21" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O21" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E22" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" t="s">
-        <v>127</v>
-      </c>
-      <c r="G22" t="s">
-        <v>128</v>
-      </c>
-      <c r="I22" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" t="s">
-        <v>132</v>
-      </c>
-      <c r="L22" t="s">
-        <v>119</v>
-      </c>
+    <row r="22" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" t="s">
-        <v>128</v>
-      </c>
-      <c r="I23" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" t="s">
-        <v>99</v>
-      </c>
-      <c r="K23" t="s">
-        <v>132</v>
-      </c>
-      <c r="L23" t="s">
-        <v>120</v>
-      </c>
+    <row r="23" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" t="s">
-        <v>98</v>
-      </c>
-      <c r="I24" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" t="s">
-        <v>99</v>
-      </c>
-      <c r="L24" t="s">
-        <v>30</v>
-      </c>
+    <row r="24" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" t="s">
-        <v>98</v>
-      </c>
-      <c r="I25" t="s">
-        <v>94</v>
-      </c>
-      <c r="J25" t="s">
-        <v>99</v>
-      </c>
-      <c r="L25" t="s">
-        <v>32</v>
-      </c>
+    <row r="25" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" t="s">
-        <v>98</v>
-      </c>
-      <c r="I26" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" t="s">
-        <v>99</v>
-      </c>
-      <c r="L26" t="s">
-        <v>33</v>
-      </c>
+    <row r="26" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" t="s">
-        <v>98</v>
-      </c>
-      <c r="I27" t="s">
-        <v>94</v>
-      </c>
-      <c r="J27" t="s">
-        <v>99</v>
-      </c>
-      <c r="L27" t="s">
-        <v>35</v>
-      </c>
+    <row r="27" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" t="s">
-        <v>98</v>
-      </c>
-      <c r="I28" t="s">
-        <v>94</v>
-      </c>
-      <c r="J28" t="s">
-        <v>99</v>
-      </c>
-      <c r="L28" t="s">
-        <v>37</v>
-      </c>
+    <row r="28" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" t="s">
-        <v>98</v>
-      </c>
-      <c r="I29" t="s">
-        <v>94</v>
-      </c>
-      <c r="J29" t="s">
-        <v>99</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>39</v>
-      </c>
+    <row r="29" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O29" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" t="s">
-        <v>98</v>
-      </c>
-      <c r="I30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J30" t="s">
-        <v>99</v>
-      </c>
-      <c r="L30" t="s">
-        <v>41</v>
-      </c>
+    <row r="30" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I31" t="s">
-        <v>94</v>
-      </c>
-      <c r="J31" t="s">
-        <v>99</v>
-      </c>
-      <c r="L31" t="s">
-        <v>43</v>
-      </c>
+    <row r="31" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" t="s">
-        <v>97</v>
-      </c>
-      <c r="G32" t="s">
-        <v>98</v>
-      </c>
-      <c r="I32" t="s">
-        <v>94</v>
-      </c>
-      <c r="J32" t="s">
-        <v>99</v>
-      </c>
-      <c r="L32" t="s">
-        <v>45</v>
-      </c>
+    <row r="32" spans="15:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" t="s">
-        <v>98</v>
-      </c>
-      <c r="I33" t="s">
-        <v>94</v>
-      </c>
-      <c r="J33" t="s">
-        <v>99</v>
-      </c>
-      <c r="L33" t="s">
-        <v>47</v>
-      </c>
+    <row r="33" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O33" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" t="s">
-        <v>94</v>
-      </c>
-      <c r="J34" t="s">
-        <v>99</v>
-      </c>
-      <c r="L34" t="s">
-        <v>49</v>
-      </c>
+    <row r="34" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" t="s">
-        <v>97</v>
-      </c>
-      <c r="G35" t="s">
-        <v>98</v>
-      </c>
-      <c r="I35" t="s">
-        <v>94</v>
-      </c>
-      <c r="J35" t="s">
-        <v>99</v>
-      </c>
-      <c r="L35" t="s">
-        <v>51</v>
-      </c>
+    <row r="35" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" t="s">
-        <v>98</v>
-      </c>
-      <c r="I36" t="s">
-        <v>94</v>
-      </c>
-      <c r="J36" t="s">
-        <v>99</v>
-      </c>
-      <c r="L36" t="s">
-        <v>53</v>
-      </c>
+    <row r="36" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" t="s">
-        <v>97</v>
-      </c>
-      <c r="G37" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" t="s">
-        <v>94</v>
-      </c>
-      <c r="J37" t="s">
-        <v>99</v>
-      </c>
-      <c r="L37" t="s">
-        <v>51</v>
-      </c>
+    <row r="37" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F38" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" t="s">
-        <v>98</v>
-      </c>
-      <c r="I38" t="s">
-        <v>94</v>
-      </c>
-      <c r="J38" t="s">
-        <v>99</v>
-      </c>
-      <c r="L38" t="s">
-        <v>53</v>
-      </c>
+    <row r="38" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O41" t="s">
         <v>92</v>
       </c>
@@ -2104,7 +1323,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O42" s="3" t="s">
         <v>74</v>
       </c>
@@ -2133,7 +1352,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O43" s="3" t="s">
         <v>75</v>
       </c>
@@ -2162,7 +1381,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O44" s="3" t="s">
         <v>76</v>
       </c>
@@ -2189,6 +1408,855 @@
       </c>
       <c r="Y44" s="3" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O46" t="s">
+        <v>67</v>
+      </c>
+      <c r="P46" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R46" t="s">
+        <v>5</v>
+      </c>
+      <c r="S46" t="s">
+        <v>127</v>
+      </c>
+      <c r="T46" t="s">
+        <v>128</v>
+      </c>
+      <c r="V46" t="s">
+        <v>94</v>
+      </c>
+      <c r="W46" t="s">
+        <v>99</v>
+      </c>
+      <c r="X46" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O47" t="s">
+        <v>68</v>
+      </c>
+      <c r="P47" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R47" t="s">
+        <v>5</v>
+      </c>
+      <c r="S47" t="s">
+        <v>127</v>
+      </c>
+      <c r="T47" t="s">
+        <v>128</v>
+      </c>
+      <c r="V47" t="s">
+        <v>94</v>
+      </c>
+      <c r="W47" t="s">
+        <v>99</v>
+      </c>
+      <c r="X47" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P48" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q48" s="1"/>
+      <c r="R48" t="s">
+        <v>8</v>
+      </c>
+      <c r="S48" t="s">
+        <v>127</v>
+      </c>
+      <c r="T48" t="s">
+        <v>128</v>
+      </c>
+      <c r="V48" t="s">
+        <v>94</v>
+      </c>
+      <c r="W48" t="s">
+        <v>99</v>
+      </c>
+      <c r="X48" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P49" s="1"/>
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O50" t="s">
+        <v>71</v>
+      </c>
+      <c r="P50" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R50" t="s">
+        <v>13</v>
+      </c>
+      <c r="S50" t="s">
+        <v>127</v>
+      </c>
+      <c r="T50" t="s">
+        <v>128</v>
+      </c>
+      <c r="V50" t="s">
+        <v>94</v>
+      </c>
+      <c r="W50" t="s">
+        <v>99</v>
+      </c>
+      <c r="X50" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P51" s="1"/>
+      <c r="R51" s="1"/>
+    </row>
+    <row r="52" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O52" t="s">
+        <v>77</v>
+      </c>
+      <c r="P52" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R52" t="s">
+        <v>78</v>
+      </c>
+      <c r="S52" t="s">
+        <v>127</v>
+      </c>
+      <c r="T52" t="s">
+        <v>128</v>
+      </c>
+      <c r="V52" t="s">
+        <v>94</v>
+      </c>
+      <c r="W52" t="s">
+        <v>99</v>
+      </c>
+      <c r="X52" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O53" t="s">
+        <v>79</v>
+      </c>
+      <c r="P53" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R53" t="s">
+        <v>18</v>
+      </c>
+      <c r="S53" t="s">
+        <v>127</v>
+      </c>
+      <c r="T53" t="s">
+        <v>128</v>
+      </c>
+      <c r="V53" t="s">
+        <v>94</v>
+      </c>
+      <c r="W53" t="s">
+        <v>99</v>
+      </c>
+      <c r="X53" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O54" t="s">
+        <v>73</v>
+      </c>
+      <c r="P54" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R54" t="s">
+        <v>20</v>
+      </c>
+      <c r="S54" t="s">
+        <v>127</v>
+      </c>
+      <c r="T54" t="s">
+        <v>128</v>
+      </c>
+      <c r="V54" t="s">
+        <v>94</v>
+      </c>
+      <c r="W54" t="s">
+        <v>99</v>
+      </c>
+      <c r="X54" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O55" t="s">
+        <v>80</v>
+      </c>
+      <c r="P55" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R55" t="s">
+        <v>81</v>
+      </c>
+      <c r="S55" t="s">
+        <v>127</v>
+      </c>
+      <c r="T55" t="s">
+        <v>128</v>
+      </c>
+      <c r="V55" t="s">
+        <v>94</v>
+      </c>
+      <c r="W55" t="s">
+        <v>99</v>
+      </c>
+      <c r="X55" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O56" t="s">
+        <v>82</v>
+      </c>
+      <c r="P56" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R56" t="s">
+        <v>83</v>
+      </c>
+      <c r="S56" t="s">
+        <v>127</v>
+      </c>
+      <c r="T56" t="s">
+        <v>128</v>
+      </c>
+      <c r="V56" t="s">
+        <v>94</v>
+      </c>
+      <c r="W56" t="s">
+        <v>99</v>
+      </c>
+      <c r="X56" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O57" t="s">
+        <v>84</v>
+      </c>
+      <c r="P57" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R57" t="s">
+        <v>85</v>
+      </c>
+      <c r="S57" t="s">
+        <v>127</v>
+      </c>
+      <c r="T57" t="s">
+        <v>128</v>
+      </c>
+      <c r="V57" t="s">
+        <v>94</v>
+      </c>
+      <c r="W57" t="s">
+        <v>99</v>
+      </c>
+      <c r="X57" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O58" t="s">
+        <v>90</v>
+      </c>
+      <c r="P58" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R58" t="s">
+        <v>25</v>
+      </c>
+      <c r="S58" t="s">
+        <v>127</v>
+      </c>
+      <c r="T58" t="s">
+        <v>128</v>
+      </c>
+      <c r="V58" t="s">
+        <v>94</v>
+      </c>
+      <c r="W58" t="s">
+        <v>99</v>
+      </c>
+      <c r="X58" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O59" t="s">
+        <v>91</v>
+      </c>
+      <c r="P59" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R59" t="s">
+        <v>27</v>
+      </c>
+      <c r="S59" t="s">
+        <v>127</v>
+      </c>
+      <c r="T59" t="s">
+        <v>128</v>
+      </c>
+      <c r="V59" t="s">
+        <v>94</v>
+      </c>
+      <c r="W59" t="s">
+        <v>99</v>
+      </c>
+      <c r="X59" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O60" t="s">
+        <v>125</v>
+      </c>
+      <c r="P60" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R60" t="s">
+        <v>86</v>
+      </c>
+      <c r="S60" t="s">
+        <v>127</v>
+      </c>
+      <c r="T60" t="s">
+        <v>128</v>
+      </c>
+      <c r="V60" t="s">
+        <v>94</v>
+      </c>
+      <c r="W60" t="s">
+        <v>99</v>
+      </c>
+      <c r="X60" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O61" t="s">
+        <v>124</v>
+      </c>
+      <c r="P61" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R61" t="s">
+        <v>87</v>
+      </c>
+      <c r="S61" t="s">
+        <v>127</v>
+      </c>
+      <c r="T61" t="s">
+        <v>128</v>
+      </c>
+      <c r="V61" t="s">
+        <v>94</v>
+      </c>
+      <c r="W61" t="s">
+        <v>99</v>
+      </c>
+      <c r="X61" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O62" t="s">
+        <v>89</v>
+      </c>
+      <c r="P62" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R62" t="s">
+        <v>88</v>
+      </c>
+      <c r="S62" t="s">
+        <v>127</v>
+      </c>
+      <c r="T62" t="s">
+        <v>128</v>
+      </c>
+      <c r="V62" t="s">
+        <v>94</v>
+      </c>
+      <c r="W62" t="s">
+        <v>99</v>
+      </c>
+      <c r="X62" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O63" t="s">
+        <v>30</v>
+      </c>
+      <c r="P63" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q63" s="1"/>
+      <c r="R63" t="s">
+        <v>31</v>
+      </c>
+      <c r="S63" t="s">
+        <v>97</v>
+      </c>
+      <c r="T63" t="s">
+        <v>98</v>
+      </c>
+      <c r="V63" t="s">
+        <v>94</v>
+      </c>
+      <c r="W63" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O64" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q64" s="1"/>
+      <c r="R64" t="s">
+        <v>31</v>
+      </c>
+      <c r="S64" t="s">
+        <v>97</v>
+      </c>
+      <c r="T64" t="s">
+        <v>98</v>
+      </c>
+      <c r="V64" t="s">
+        <v>94</v>
+      </c>
+      <c r="W64" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O65" t="s">
+        <v>33</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q65" s="1"/>
+      <c r="R65" t="s">
+        <v>34</v>
+      </c>
+      <c r="S65" t="s">
+        <v>97</v>
+      </c>
+      <c r="T65" t="s">
+        <v>98</v>
+      </c>
+      <c r="V65" t="s">
+        <v>94</v>
+      </c>
+      <c r="W65" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O66" t="s">
+        <v>35</v>
+      </c>
+      <c r="P66" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q66" s="1"/>
+      <c r="R66" t="s">
+        <v>36</v>
+      </c>
+      <c r="S66" t="s">
+        <v>97</v>
+      </c>
+      <c r="T66" t="s">
+        <v>98</v>
+      </c>
+      <c r="V66" t="s">
+        <v>94</v>
+      </c>
+      <c r="W66" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O67" t="s">
+        <v>37</v>
+      </c>
+      <c r="P67" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q67" s="1"/>
+      <c r="R67" t="s">
+        <v>38</v>
+      </c>
+      <c r="S67" t="s">
+        <v>97</v>
+      </c>
+      <c r="T67" t="s">
+        <v>98</v>
+      </c>
+      <c r="V67" t="s">
+        <v>94</v>
+      </c>
+      <c r="W67" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O68" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P68" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q68" s="1"/>
+      <c r="R68" t="s">
+        <v>40</v>
+      </c>
+      <c r="S68" t="s">
+        <v>97</v>
+      </c>
+      <c r="T68" t="s">
+        <v>98</v>
+      </c>
+      <c r="V68" t="s">
+        <v>94</v>
+      </c>
+      <c r="W68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y68" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O69" t="s">
+        <v>41</v>
+      </c>
+      <c r="P69" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q69" s="1"/>
+      <c r="R69" t="s">
+        <v>42</v>
+      </c>
+      <c r="S69" t="s">
+        <v>97</v>
+      </c>
+      <c r="T69" t="s">
+        <v>98</v>
+      </c>
+      <c r="V69" t="s">
+        <v>94</v>
+      </c>
+      <c r="W69" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O70" t="s">
+        <v>43</v>
+      </c>
+      <c r="P70" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q70" s="1"/>
+      <c r="R70" t="s">
+        <v>44</v>
+      </c>
+      <c r="S70" t="s">
+        <v>97</v>
+      </c>
+      <c r="T70" t="s">
+        <v>98</v>
+      </c>
+      <c r="V70" t="s">
+        <v>94</v>
+      </c>
+      <c r="W70" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O71" t="s">
+        <v>45</v>
+      </c>
+      <c r="P71" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q71" s="1"/>
+      <c r="R71" t="s">
+        <v>46</v>
+      </c>
+      <c r="S71" t="s">
+        <v>97</v>
+      </c>
+      <c r="T71" t="s">
+        <v>98</v>
+      </c>
+      <c r="V71" t="s">
+        <v>94</v>
+      </c>
+      <c r="W71" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O72" t="s">
+        <v>47</v>
+      </c>
+      <c r="P72" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q72" s="1"/>
+      <c r="R72" t="s">
+        <v>48</v>
+      </c>
+      <c r="S72" t="s">
+        <v>97</v>
+      </c>
+      <c r="T72" t="s">
+        <v>98</v>
+      </c>
+      <c r="V72" t="s">
+        <v>94</v>
+      </c>
+      <c r="W72" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O73" t="s">
+        <v>49</v>
+      </c>
+      <c r="P73" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q73" s="1"/>
+      <c r="R73" t="s">
+        <v>50</v>
+      </c>
+      <c r="S73" t="s">
+        <v>97</v>
+      </c>
+      <c r="T73" t="s">
+        <v>98</v>
+      </c>
+      <c r="V73" t="s">
+        <v>94</v>
+      </c>
+      <c r="W73" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O74" t="s">
+        <v>51</v>
+      </c>
+      <c r="P74" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q74" s="1"/>
+      <c r="R74" t="s">
+        <v>52</v>
+      </c>
+      <c r="S74" t="s">
+        <v>97</v>
+      </c>
+      <c r="T74" t="s">
+        <v>98</v>
+      </c>
+      <c r="V74" t="s">
+        <v>94</v>
+      </c>
+      <c r="W74" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O75" t="s">
+        <v>53</v>
+      </c>
+      <c r="P75" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q75" s="1"/>
+      <c r="R75" t="s">
+        <v>54</v>
+      </c>
+      <c r="S75" t="s">
+        <v>97</v>
+      </c>
+      <c r="T75" t="s">
+        <v>98</v>
+      </c>
+      <c r="V75" t="s">
+        <v>94</v>
+      </c>
+      <c r="W75" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O76" t="s">
+        <v>51</v>
+      </c>
+      <c r="P76" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q76" s="1"/>
+      <c r="R76" t="s">
+        <v>52</v>
+      </c>
+      <c r="S76" t="s">
+        <v>97</v>
+      </c>
+      <c r="T76" t="s">
+        <v>98</v>
+      </c>
+      <c r="V76" t="s">
+        <v>94</v>
+      </c>
+      <c r="W76" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="15:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O77" t="s">
+        <v>53</v>
+      </c>
+      <c r="P77" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q77" s="1"/>
+      <c r="R77" t="s">
+        <v>54</v>
+      </c>
+      <c r="S77" t="s">
+        <v>97</v>
+      </c>
+      <c r="T77" t="s">
+        <v>98</v>
+      </c>
+      <c r="V77" t="s">
+        <v>94</v>
+      </c>
+      <c r="W77" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>